<commit_message>
DHW: update input files
</commit_message>
<xml_diff>
--- a/Input/SimInput.xlsx
+++ b/Input/SimInput.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A87D6F4-2A73-44C8-8680-0CA2ABC44448}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589A94E5-6B41-4040-BAF2-83728264A87D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
   <si>
     <t>Input files</t>
   </si>
@@ -248,6 +248,21 @@
   </si>
   <si>
     <t>.json</t>
+  </si>
+  <si>
+    <t>DHW calculation (only residential)</t>
+  </si>
+  <si>
+    <t>Volume calculation</t>
+  </si>
+  <si>
+    <t>Time range</t>
+  </si>
+  <si>
+    <t>Static</t>
+  </si>
+  <si>
+    <t>Time step</t>
   </si>
 </sst>
 </file>
@@ -490,7 +505,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,17 +536,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -804,27 +819,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="31.5703125" customWidth="1"/>
     <col min="4" max="4" width="12" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -852,7 +867,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="12" t="str">
-        <f t="shared" ref="D3:D10" si="0">CONCATENATE(C3,B3)</f>
+        <f t="shared" ref="D3:D6" si="0">CONCATENATE(C3,B3)</f>
         <v>Envelopes.xlsx</v>
       </c>
     </row>
@@ -941,456 +956,495 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="28"/>
+      <c r="D10" s="20"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="25">
         <v>2020</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="26"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="29">
         <v>7</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="30"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="26"/>
+      <c r="C16" s="30"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="29">
         <v>1</v>
       </c>
-      <c r="C17" s="26"/>
+      <c r="C17" s="30"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="27">
         <v>8760</v>
       </c>
-      <c r="C18" s="24"/>
+      <c r="C18" s="28"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="26"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="25">
+      <c r="B20" s="29">
         <v>167</v>
       </c>
-      <c r="C20" s="26"/>
+      <c r="C20" s="30"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="29">
         <v>504</v>
       </c>
-      <c r="C21" s="26"/>
+      <c r="C21" s="30"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="25">
+      <c r="B22" s="29">
         <v>4681</v>
       </c>
-      <c r="C22" s="26"/>
+      <c r="C22" s="30"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B23" s="29">
         <v>5017</v>
       </c>
-      <c r="C23" s="26"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="29">
         <v>168</v>
       </c>
-      <c r="C24" s="26"/>
+      <c r="C24" s="30"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="26"/>
+      <c r="C25" s="30"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="26"/>
+      <c r="C26" s="30"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="24"/>
+      <c r="C27" s="28"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="25">
         <v>8</v>
       </c>
-      <c r="C28" s="22"/>
+      <c r="C28" s="26"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="25">
+      <c r="B29" s="29">
         <v>3</v>
       </c>
-      <c r="C29" s="26"/>
+      <c r="C29" s="30"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="24"/>
+      <c r="C30" s="28"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="22"/>
+      <c r="C31" s="26"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="25">
+      <c r="B32" s="29">
         <v>80</v>
       </c>
-      <c r="C32" s="26"/>
+      <c r="C32" s="30"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B33" s="29">
         <v>100</v>
       </c>
-      <c r="C33" s="26"/>
+      <c r="C33" s="30"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B34" s="29">
         <v>80</v>
       </c>
-      <c r="C34" s="26"/>
+      <c r="C34" s="30"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="27">
         <v>0</v>
       </c>
-      <c r="C35" s="24"/>
+      <c r="C35" s="28"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="17"/>
+      <c r="A36" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="26"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="30"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="28"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="17"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="19">
-        <v>530000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" s="19">
-        <v>800</v>
-      </c>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="19">
-        <v>3280</v>
+        <v>60</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="19">
+        <v>530000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="19">
+      <c r="C44" s="19">
         <v>800</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
-        <v>49</v>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>46</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C45" s="19">
-        <v>17</v>
+        <v>3280</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C46" s="19">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>66</v>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
+        <v>48</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C47" s="19">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C48" s="19">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
-        <v>51</v>
+      <c r="A49" t="s">
+        <v>50</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C49" s="19">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="18" t="s">
-        <v>67</v>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>66</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C50" s="19">
-        <v>5</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C51" s="19">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C52" s="19">
-        <v>114</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C53" s="19">
-        <v>88</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C54" s="19">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C55" s="19">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C56" s="19">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C57" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C58" s="19">
-        <v>64</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="19">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B62" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C59" s="19">
+      <c r="C62" s="19">
         <v>2283</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="28">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="B14:C14"/>
@@ -1407,17 +1461,8 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{BC996E9F-B116-4051-82FE-1C81AE5B949F}">
       <formula1>".json,.geojson"</formula1>
     </dataValidation>
@@ -1427,6 +1472,12 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{C4529080-CD8B-44E7-82F8-8FA761746EC2}">
       <formula1>"Daily,Yearly"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37:C37" xr:uid="{076377A6-6393-4592-BF3D-8BDD83EDB19B}">
+      <formula1>"Static,ISO 11300-2"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38:C38" xr:uid="{D1172021-BF62-4504-B30B-2AB94679A070}">
+      <formula1>"Time step,Year"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed error on geojson index in city object
</commit_message>
<xml_diff>
--- a/Input/SimInput.xlsx
+++ b/Input/SimInput.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CF18DA-03F6-4C12-A876-8E3AC85B3503}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDE113B-6E0D-4F9E-87D7-3163BFAEF7CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autore</author>
+    <author>Author</author>
   </authors>
   <commentList>
     <comment ref="B39" authorId="0" shapeId="0" xr:uid="{2DA80E13-9FAD-4266-A48F-295317104571}">
@@ -35,7 +35,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Autore:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -559,25 +559,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -598,9 +586,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,12 +893,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1018,256 +1018,256 @@
       <c r="D10" s="20"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="30">
         <v>2020</v>
       </c>
-      <c r="C14" s="26"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="22">
         <v>7</v>
       </c>
-      <c r="C15" s="24"/>
+      <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="24"/>
+      <c r="C16" s="23"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="22">
         <v>1</v>
       </c>
-      <c r="C17" s="24"/>
+      <c r="C17" s="23"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="32">
         <v>8760</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="33"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="26"/>
+      <c r="C19" s="31"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="22">
         <v>167</v>
       </c>
-      <c r="C20" s="24"/>
+      <c r="C20" s="23"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="22">
         <v>504</v>
       </c>
-      <c r="C21" s="24"/>
+      <c r="C21" s="23"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="22">
         <v>4681</v>
       </c>
-      <c r="C22" s="24"/>
+      <c r="C22" s="23"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="22">
         <v>5017</v>
       </c>
-      <c r="C23" s="24"/>
+      <c r="C23" s="23"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="22">
         <v>168</v>
       </c>
-      <c r="C24" s="24"/>
+      <c r="C24" s="23"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="24"/>
+      <c r="C25" s="23"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="24"/>
+      <c r="C26" s="23"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="22"/>
+      <c r="C27" s="33"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="25">
+      <c r="B28" s="30">
         <v>8</v>
       </c>
-      <c r="C28" s="26"/>
+      <c r="C28" s="31"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B29" s="22">
         <v>3</v>
       </c>
-      <c r="C29" s="24"/>
+      <c r="C29" s="23"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="22"/>
+      <c r="C30" s="33"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="26"/>
+      <c r="C31" s="31"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B32" s="22">
         <v>80</v>
       </c>
-      <c r="C32" s="24"/>
+      <c r="C32" s="23"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B33" s="22">
         <v>100</v>
       </c>
-      <c r="C33" s="24"/>
+      <c r="C33" s="23"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="23">
+      <c r="B34" s="22">
         <v>80</v>
       </c>
-      <c r="C34" s="24"/>
+      <c r="C34" s="23"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="22">
         <v>0</v>
       </c>
-      <c r="C35" s="24"/>
+      <c r="C35" s="23"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="26"/>
+      <c r="C36" s="31"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="24"/>
+      <c r="C37" s="23"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="24"/>
+      <c r="C38" s="23"/>
       <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="29"/>
+      <c r="C39" s="25"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="17"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1502,6 +1502,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B39:C39"/>
@@ -1518,19 +1531,6 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B28:C28"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{BC996E9F-B116-4051-82FE-1C81AE5B949F}">

</xml_diff>

<commit_message>
Fixed error in index of json city object buildings
</commit_message>
<xml_diff>
--- a/Input/SimInput.xlsx
+++ b/Input/SimInput.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDE113B-6E0D-4F9E-87D7-3163BFAEF7CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A15B11D-7FEE-469B-B003-858B9A2EB3AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
   <si>
     <t>Input files</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Envelopes</t>
   </si>
   <si>
-    <t>ScheduleSemp</t>
-  </si>
-  <si>
     <t>PlantsList</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>End-uses mode</t>
   </si>
   <si>
-    <t>Daily</t>
-  </si>
-  <si>
     <t>DHW calculation (only residential)</t>
   </si>
   <si>
@@ -293,16 +287,22 @@
     <t>Residenziale</t>
   </si>
   <si>
-    <t>.geojson</t>
-  </si>
-  <si>
-    <t>PiovegoRestricted</t>
-  </si>
-  <si>
-    <t>geojson</t>
-  </si>
-  <si>
     <t>Static</t>
+  </si>
+  <si>
+    <t>PaduaRestricted</t>
+  </si>
+  <si>
+    <t>cityjson</t>
+  </si>
+  <si>
+    <t>.json</t>
+  </si>
+  <si>
+    <t>ScheduleComp</t>
+  </si>
+  <si>
+    <t>Yearly</t>
   </si>
 </sst>
 </file>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,11 +938,11 @@
         <v>8</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="D4" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>ScheduleSemp.xlsx</v>
+        <v>ScheduleComp.xlsx</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -953,7 +953,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="12" t="str">
         <f t="shared" si="0"/>
@@ -965,14 +965,14 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D6" s="12" t="str">
         <f t="shared" si="0"/>
-        <v>PiovegoRestricted.geojson</v>
+        <v>PaduaRestricted.json</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -990,28 +990,28 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="9" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D8" s="12" t="str">
         <f>C8</f>
-        <v>Daily</v>
+        <v>Yearly</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D9" s="13" t="str">
         <f>C9</f>
-        <v>geojson</v>
+        <v>cityjson</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1019,14 +1019,14 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="30">
         <v>2020</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="22">
         <v>7</v>
@@ -1044,16 +1044,16 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="23"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="22">
         <v>1</v>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="32">
         <v>8760</v>
@@ -1071,16 +1071,16 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="31"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="22">
         <v>167</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="22">
         <v>504</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="22">
         <v>4681</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="22">
         <v>5017</v>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="22">
         <v>168</v>
@@ -1125,34 +1125,34 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="23"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="23"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="33"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="30">
         <v>8</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="22">
         <v>3</v>
@@ -1170,25 +1170,25 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" s="33"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="31"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="22">
         <v>80</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="22">
         <v>100</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="22">
         <v>80</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" s="22">
         <v>0</v>
@@ -1224,38 +1224,38 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="30" t="s">
-        <v>39</v>
+        <v>71</v>
+      </c>
+      <c r="B36" s="30" t="b">
+        <v>0</v>
       </c>
       <c r="C36" s="31"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C37" s="23"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="23"/>
       <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" s="25"/>
     </row>
@@ -1264,28 +1264,28 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="19">
         <v>530000</v>
@@ -1293,10 +1293,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" s="19">
         <v>800</v>
@@ -1304,10 +1304,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="19">
         <v>3280</v>
@@ -1315,10 +1315,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C47" s="19">
         <v>800</v>
@@ -1326,10 +1326,10 @@
     </row>
     <row r="48" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C48" s="19">
         <v>5</v>
@@ -1337,10 +1337,10 @@
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" s="19">
         <v>17</v>
@@ -1348,10 +1348,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" s="19">
         <v>0.85</v>
@@ -1359,10 +1359,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C51" s="19">
         <v>0.15</v>
@@ -1370,10 +1370,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C52" s="19">
         <v>2</v>
@@ -1381,10 +1381,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" s="19">
         <v>0.16</v>
@@ -1392,10 +1392,10 @@
     </row>
     <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C54" s="19">
         <v>5</v>
@@ -1403,10 +1403,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C55" s="19">
         <v>655</v>
@@ -1414,10 +1414,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C56" s="19">
         <v>114</v>
@@ -1425,10 +1425,10 @@
     </row>
     <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C57" s="19">
         <v>88</v>
@@ -1436,10 +1436,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C58" s="19">
         <v>25</v>
@@ -1447,10 +1447,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" s="19">
         <v>13</v>
@@ -1458,10 +1458,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C60" s="19">
         <v>105</v>
@@ -1469,10 +1469,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C61" s="19">
         <v>1</v>
@@ -1480,10 +1480,10 @@
     </row>
     <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" s="19">
         <v>64</v>
@@ -1491,10 +1491,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C63" s="19">
         <v>2283</v>

</xml_diff>